<commit_message>
modification of logging. Addition of local and global logs, adding warnings and errors to the table
</commit_message>
<xml_diff>
--- a/track_day1_example/results_input.xlsx
+++ b/track_day1_example/results_input.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tinc9\Documents\sportident\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tinc9\Documents\sportident\track_day1_example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A70658-D399-4F8B-ACC9-785156CEBAC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B0487B8-87D3-4DAB-90E8-EC89BF82DB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Ekipe</t>
   </si>
@@ -45,9 +45,6 @@
     <t>mrtvi cas skupno</t>
   </si>
   <si>
-    <t>prekoracitve casovnic</t>
-  </si>
-  <si>
     <t>Vrstni red Ktjev</t>
   </si>
   <si>
@@ -64,16 +61,105 @@
   </si>
   <si>
     <t>SIID</t>
+  </si>
+  <si>
+    <t>KT1</t>
+  </si>
+  <si>
+    <t>KT2</t>
+  </si>
+  <si>
+    <t>KT3</t>
+  </si>
+  <si>
+    <t>KT4</t>
+  </si>
+  <si>
+    <t>KT5</t>
+  </si>
+  <si>
+    <t>KT6</t>
+  </si>
+  <si>
+    <t>KT7</t>
+  </si>
+  <si>
+    <t>KT8</t>
+  </si>
+  <si>
+    <t>KT9</t>
+  </si>
+  <si>
+    <t>KT10</t>
+  </si>
+  <si>
+    <t>KT11</t>
+  </si>
+  <si>
+    <t>KT12</t>
+  </si>
+  <si>
+    <t>KT13</t>
+  </si>
+  <si>
+    <t>KT14</t>
+  </si>
+  <si>
+    <t>KT15</t>
+  </si>
+  <si>
+    <t>KT16</t>
+  </si>
+  <si>
+    <t>KT17</t>
+  </si>
+  <si>
+    <t>KT18</t>
+  </si>
+  <si>
+    <t>KT19</t>
+  </si>
+  <si>
+    <t>KT20</t>
+  </si>
+  <si>
+    <t># KTjev iz casovnice</t>
+  </si>
+  <si>
+    <t>Opozorila</t>
+  </si>
+  <si>
+    <t>Napake</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -88,18 +174,16 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -107,29 +191,20 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -143,6 +218,49 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{42F5300F-5F13-419C-958E-095C704C48E1}" name="Table1" displayName="Table1" ref="A1:AH17" totalsRowShown="0">
+  <autoFilter ref="A1:AH17" xr:uid="{42F5300F-5F13-419C-958E-095C704C48E1}"/>
+  <tableColumns count="34">
+    <tableColumn id="1" xr3:uid="{C2F6D500-5FCE-45C6-BA89-2FAB7EB1D8A0}" name="Ekipe"/>
+    <tableColumn id="2" xr3:uid="{042EF954-C35A-4AAD-ACB0-7C8EBBEB4197}" name="SIID"/>
+    <tableColumn id="3" xr3:uid="{A791CA10-5F8A-4BB3-8070-76B7E6661A80}" name="Start"/>
+    <tableColumn id="4" xr3:uid="{ED07D189-608D-4B21-B03E-EF5D86EF5B2F}" name="Cilj"/>
+    <tableColumn id="5" xr3:uid="{FCC1B82F-62DC-4BFF-8505-65F4823BA6AB}" name="Skupni cas (brez mrtvega)"/>
+    <tableColumn id="6" xr3:uid="{9154AFD9-412C-4EB4-9EC6-E61CB3AF8AED}" name="Mrtvi cas opisno"/>
+    <tableColumn id="7" xr3:uid="{16D8F316-71AD-4B34-B542-D13955D90BCF}" name="mrtvi cas skupno"/>
+    <tableColumn id="8" xr3:uid="{98C1BB3D-FB6D-48A2-AE09-269C6756EBB2}" name="skupni cas final" dataCellStyle="Good"/>
+    <tableColumn id="9" xr3:uid="{1423F76C-C4ED-4ED2-96A6-D679DB657E88}" name="Vrstni red Ktjev"/>
+    <tableColumn id="10" xr3:uid="{BD325A9F-E61A-423E-B76A-6C41BFA6A473}" name="# KTjev iz casovnice"/>
+    <tableColumn id="11" xr3:uid="{CA9DCF54-3A04-40F4-A38A-F71B616D88FC}" name="Stevilo Ktjev" dataCellStyle="Good"/>
+    <tableColumn id="12" xr3:uid="{55300F48-C1A6-4025-B4AF-B50992A89F78}" name="hitrostna cas" dataCellStyle="Good"/>
+    <tableColumn id="13" xr3:uid="{AF3DB0EE-A7D4-4535-821D-91051D677508}" name="Opozorila" dataCellStyle="Bad"/>
+    <tableColumn id="14" xr3:uid="{42A084C5-AEA5-424B-94AA-BD175A8F12D8}" name="Napake"/>
+    <tableColumn id="15" xr3:uid="{334F33DF-48B2-448B-9C09-DD1D884AF02D}" name="KT1"/>
+    <tableColumn id="16" xr3:uid="{FBE56044-21B8-4EB6-AC61-308F57725F34}" name="KT2"/>
+    <tableColumn id="17" xr3:uid="{4723C77A-91A1-41F4-A0F2-4054CAD5C1D4}" name="KT3"/>
+    <tableColumn id="18" xr3:uid="{047F12DD-780A-4997-835A-EA0CF850E4AE}" name="KT4"/>
+    <tableColumn id="19" xr3:uid="{096E7EB3-5B4F-4582-A1B8-F97474C2EE3C}" name="KT5"/>
+    <tableColumn id="20" xr3:uid="{490CF523-07FD-4CEF-A67C-B05FE1CA93FE}" name="KT6"/>
+    <tableColumn id="21" xr3:uid="{55B07E6F-262E-4BD4-A9F0-007BD2E834F3}" name="KT7"/>
+    <tableColumn id="22" xr3:uid="{F11C537E-60C7-490E-95AF-0DFDB00A84F8}" name="KT8"/>
+    <tableColumn id="23" xr3:uid="{F55CE1A7-EE84-458E-AD20-B3A93B47766E}" name="KT9"/>
+    <tableColumn id="24" xr3:uid="{33CC7AAD-BB32-4B2F-B7C2-37EA888FC4FE}" name="KT10"/>
+    <tableColumn id="25" xr3:uid="{89A1C878-3867-433E-9D4A-11A0C7F2B424}" name="KT11"/>
+    <tableColumn id="26" xr3:uid="{DCD2A804-C99C-468D-9AFA-1589A26DA997}" name="KT12"/>
+    <tableColumn id="27" xr3:uid="{9117B5D2-84A9-463C-8FA2-4E51102CACCA}" name="KT13"/>
+    <tableColumn id="28" xr3:uid="{24569E07-5AE8-4B41-AA1C-216F48CDFD1D}" name="KT14"/>
+    <tableColumn id="29" xr3:uid="{F661326D-7731-4F9B-9270-32FBBE926F8E}" name="KT15"/>
+    <tableColumn id="30" xr3:uid="{6FBE27FD-E469-4951-9317-C7EE730F5E46}" name="KT16"/>
+    <tableColumn id="31" xr3:uid="{79CC755F-C009-4999-9FA2-FF2FFD146C3C}" name="KT17"/>
+    <tableColumn id="32" xr3:uid="{5C4B63FF-357C-4331-8F11-21AED59F869F}" name="KT18"/>
+    <tableColumn id="33" xr3:uid="{17497417-41D1-4F39-B146-6B4F1EE1C641}" name="KT19"/>
+    <tableColumn id="34" xr3:uid="{3E7BF403-8699-4D7F-832D-C4875103EC3F}" name="KT20"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -408,30 +526,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:AH18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="22.453125" customWidth="1"/>
-    <col min="6" max="6" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.90625" customWidth="1"/>
-    <col min="9" max="9" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.453125" customWidth="1"/>
-    <col min="12" max="12" width="12.26953125" customWidth="1"/>
+    <col min="5" max="5" width="24.453125" customWidth="1"/>
+    <col min="6" max="6" width="16.54296875" customWidth="1"/>
+    <col min="7" max="7" width="16.90625" customWidth="1"/>
+    <col min="8" max="8" width="15.7265625" customWidth="1"/>
+    <col min="9" max="9" width="16" customWidth="1"/>
+    <col min="10" max="10" width="19.26953125" customWidth="1"/>
+    <col min="11" max="12" width="13.54296875" customWidth="1"/>
+    <col min="13" max="13" width="11.08984375" customWidth="1"/>
+    <col min="14" max="14" width="9.26953125" customWidth="1"/>
+    <col min="15" max="23" width="5.90625" customWidth="1"/>
+    <col min="24" max="34" width="6.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -448,150 +569,291 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
-        <v>8</v>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="I1" t="s">
         <v>6</v>
       </c>
       <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T1" t="s">
+        <v>17</v>
+      </c>
+      <c r="U1" t="s">
+        <v>18</v>
+      </c>
+      <c r="V1" t="s">
+        <v>19</v>
+      </c>
+      <c r="W1" t="s">
+        <v>20</v>
+      </c>
+      <c r="X1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>101</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>2103529</v>
       </c>
-      <c r="C2" s="4"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="H2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>102</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3">
         <v>2103519</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="H3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>103</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4">
         <v>2052383</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="H4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>104</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5">
         <v>1401586</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="H5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>105</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6">
         <v>2078588</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="H6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>106</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7">
         <v>2103521</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="H7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>107</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8">
         <v>1401547</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="H8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>108</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9">
         <v>1401596</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="H9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>109</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10">
         <v>1401588</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="H10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>110</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11">
         <v>1401503</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="H11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="1"/>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>111</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
         <v>1401597</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="H12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="1"/>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>112</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13">
         <v>2069823</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="H13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="1"/>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>113</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14">
         <v>1401501</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="H14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="1"/>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>114</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15">
         <v>2041793</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="3">
+      <c r="H15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="1"/>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A16">
         <v>115</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16">
         <v>1401544</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>11</v>
+      <c r="H16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="1"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>116</v>
+      </c>
+      <c r="B17">
+        <v>1231231</v>
+      </c>
+      <c r="H17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="1"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>